<commit_message>
adjust alignment for printing
</commit_message>
<xml_diff>
--- a/doc/APIs_LKHv1.xlsx
+++ b/doc/APIs_LKHv1.xlsx
@@ -1,32 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="188" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView windowWidth="18500" windowHeight="9680"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:G22</definedName>
+  </definedNames>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
   <si>
     <r>
-      <t xml:space="preserve">API</t>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="0"/>
+      </rPr>
+      <t>API</t>
     </r>
     <r>
       <rPr>
-        <rFont val="WenQuanYi Zen Hei"/>
+        <sz val="10"/>
+        <rFont val="宋体"/>
         <family val="2"/>
-        <sz val="10"/>
+        <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">类别</t>
+      <t>类别</t>
     </r>
   </si>
   <si>
@@ -51,7 +61,8 @@
     <t>newUser</t>
   </si>
   <si>
-    <t>email, username, passwd, imagedata gender</t>
+    <t>email, username, passwd, image data,
+gender</t>
   </si>
   <si>
     <t>success, auth_token</t>
@@ -109,32 +120,18 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">username, gender, </t>
+      <t>username, gender,</t>
     </r>
     <r>
       <rPr>
-        <rFont val="WenQuanYi Zen Hei"/>
+        <sz val="10"/>
+        <rFont val="宋体"/>
         <family val="2"/>
-        <sz val="10"/>
+        <charset val="0"/>
       </rPr>
-      <t xml:space="preserve">以后可能会有</t>
+      <t>DateOfBirth,
+auth_token, pair</t>
     </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">DateOfBirth, auth_token, pair, </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="WenQuanYi Zen Hei"/>
-        <family val="2"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">各种</t>
-    </r>
   </si>
   <si>
     <t>GEP</t>
@@ -158,7 +155,8 @@
     <t>newPair</t>
   </si>
   <si>
-    <t>username1, username2, auth_token1, auth_token2</t>
+    <t>username1, username2, auth_token1, 
+auth_token2</t>
   </si>
   <si>
     <t>success, pairId</t>
@@ -173,7 +171,7 @@
     <t>pairId</t>
   </si>
   <si>
-    <t>http://URL/pair/pairId</t>
+    <t>http://URL/pair/pId</t>
   </si>
   <si>
     <t>removePair</t>
@@ -200,7 +198,8 @@
     <t>username, auth_token</t>
   </si>
   <si>
-    <t>success, firstMoodId, lastMoodId, comment Text</t>
+    <t>success, firstMoodId, lastMoodId,
+comment Text</t>
   </si>
   <si>
     <t>getMood</t>
@@ -234,34 +233,48 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
+      <charset val="0"/>
     </font>
     <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="4"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <family val="2"/>
+      <charset val="0"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <charset val="0"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
-      <name val="WenQuanYi Zen Hei"/>
+      <sz val="10"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -272,8 +285,15 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -281,372 +301,716 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="9">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Currency [0]" xfId="1"/>
+    <cellStyle name="货币[0]" xfId="2" builtinId="7"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔" xfId="4" builtinId="3"/>
+    <cellStyle name="货币" xfId="5" builtinId="4"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="Comma [0]" xfId="7"/>
+    <cellStyle name="千位分隔[0]" xfId="8" builtinId="6"/>
   </cellStyles>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5265C0" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5265C0" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5265C0" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="000000" lon="000000" rev="000000"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="000000" lon="000000" rev="124F80"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:satMod val="350000"/>
+                <a:shade val="99000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="_h" fmla="val 21600"/>
+            <a:gd name="_w" fmla="val 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:pathLst>
+            <a:path w="21600" h="21600"/>
+          </a:pathLst>
+        </a:custGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:srgbClr val="9CBEE0"/>
+            </a:gs>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="739CC3"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="200000"/>
+        </a:ln>
+      </a:spPr>
+      <a:bodyPr/>
+      <a:lstStyle/>
+    </a:spDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C22" activeCellId="0" pane="topLeft" sqref="C22:C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="11.25" outlineLevelCol="5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" width="11.5238095238095"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="42.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="38.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="26.5714285714286" customWidth="1"/>
+    <col min="6" max="1025" width="11.5238095238095"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
+    <row r="2" ht="22.5">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
-      <c r="B3" s="0" t="s">
+    <row r="3">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
-      <c r="B4" s="0" t="s">
+    <row r="4">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="B5" s="0" t="s">
+    <row r="5">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="6">
-      <c r="B6" s="0" t="s">
+    <row r="6" ht="22.5">
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
-      <c r="B8" s="0" t="s">
+    <row r="8">
+      <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
-      <c r="A9" s="0" t="s">
+    <row r="9">
+      <c r="A9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
-      <c r="B10" s="0" t="s">
+    <row r="10" ht="22.5">
+      <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
-      <c r="B11" s="0" t="s">
+    <row r="11">
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="B12" s="0" t="s">
+    <row r="12">
+      <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="B14" s="0" t="s">
+    <row r="14">
+      <c r="B14" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
-      <c r="A15" s="0" t="s">
+    <row r="15">
+      <c r="A15" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
-      <c r="B16" s="0" t="s">
+    <row r="16" ht="22.5">
+      <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
-      <c r="B17" s="0" t="s">
+    <row r="17">
+      <c r="B17" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
-      <c r="B19" s="0" t="s">
+    <row r="19">
+      <c r="B19" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
-      <c r="A20" s="0" t="s">
+    <row r="20">
+      <c r="A20" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  <pageMargins left="0.786805555555556" right="0.786805555555556" top="1.05069444444444" bottom="1.05069444444444" header="0.786805555555556" footer="0.786805555555556"/>
+  <pageSetup paperSize="9" scale="75" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>